<commit_message>
Updated data to contain units.
</commit_message>
<xml_diff>
--- a/data/eeu_data.xlsx
+++ b/data/eeu_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/ReboundTools/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF27230B-FEF8-BF4E-8D9A-B5212EDE3ECB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F56CE73F-FB32-5648-B22E-E1AD15905E83}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="23180" yWindow="460" windowWidth="26260" windowHeight="16940" xr2:uid="{7964B245-1BB5-784B-946F-34F7FEF70238}"/>
   </bookViews>
@@ -30,7 +30,106 @@
     <author>Matthew Heun</author>
   </authors>
   <commentList>
-    <comment ref="E2" authorId="0" shapeId="0" xr:uid="{9482D8EB-43D3-CD42-B9A3-577AD33D043C}">
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{177A5939-9C5C-134F-8638-CA4D7AC90D6E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This is the unit of the numerator of the efficiency terms.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{E7917100-B885-C647-B060-CE8FA6C0FA9F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This is the unit of denominator of the efficiency terms.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{2E9F2B67-4158-6D4C-9AF8-868A6C525FDC}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This unit conversion factor translates from energy engineering units to MJ.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G2" authorId="0" shapeId="0" xr:uid="{9482D8EB-43D3-CD42-B9A3-577AD33D043C}">
       <text>
         <r>
           <rPr>
@@ -63,7 +162,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F2" authorId="0" shapeId="0" xr:uid="{142CF5A0-F2F7-6049-8D23-3DC70BA56F2B}">
+    <comment ref="H2" authorId="0" shapeId="0" xr:uid="{142CF5A0-F2F7-6049-8D23-3DC70BA56F2B}">
       <text>
         <r>
           <rPr>
@@ -96,40 +195,40 @@
         </r>
       </text>
     </comment>
-    <comment ref="H2" authorId="0" shapeId="0" xr:uid="{212DB243-4B09-8641-8DD9-2C5771F409BE}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Matthew Heun:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>$/MJ</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I2" authorId="0" shapeId="0" xr:uid="{BD5F855E-F716-1C40-9BD9-51470AF65E6E}">
+    <comment ref="J2" authorId="0" shapeId="0" xr:uid="{212DB243-4B09-8641-8DD9-2C5771F409BE}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>$/gal</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K2" authorId="0" shapeId="0" xr:uid="{BD5F855E-F716-1C40-9BD9-51470AF65E6E}">
       <text>
         <r>
           <rPr>
@@ -162,7 +261,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J2" authorId="0" shapeId="0" xr:uid="{724ED12C-E3B7-174A-AED0-FF81928555B3}">
+    <comment ref="L2" authorId="0" shapeId="0" xr:uid="{724ED12C-E3B7-174A-AED0-FF81928555B3}">
       <text>
         <r>
           <rPr>
@@ -195,7 +294,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N2" authorId="0" shapeId="0" xr:uid="{2E11DCDD-2255-D142-98F1-B4F74C45A04F}">
+    <comment ref="P2" authorId="0" shapeId="0" xr:uid="{2E11DCDD-2255-D142-98F1-B4F74C45A04F}">
       <text>
         <r>
           <rPr>
@@ -228,7 +327,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O2" authorId="0" shapeId="0" xr:uid="{30C499C2-FCE1-5541-A599-047491F4BB43}">
+    <comment ref="Q2" authorId="0" shapeId="0" xr:uid="{30C499C2-FCE1-5541-A599-047491F4BB43}">
       <text>
         <r>
           <rPr>
@@ -261,7 +360,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P2" authorId="0" shapeId="0" xr:uid="{15643D2B-90F6-2E4E-923B-C7BAE01F5865}">
+    <comment ref="R2" authorId="0" shapeId="0" xr:uid="{15643D2B-90F6-2E4E-923B-C7BAE01F5865}">
       <text>
         <r>
           <rPr>
@@ -294,7 +393,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q2" authorId="0" shapeId="0" xr:uid="{C60C194C-E6D8-714B-8103-E2256CEE5592}">
+    <comment ref="S2" authorId="0" shapeId="0" xr:uid="{C60C194C-E6D8-714B-8103-E2256CEE5592}">
       <text>
         <r>
           <rPr>
@@ -327,7 +426,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R2" authorId="0" shapeId="0" xr:uid="{FF3DF81E-1DB0-BC43-B287-7EE6D75FE27A}">
+    <comment ref="T2" authorId="0" shapeId="0" xr:uid="{FF3DF81E-1DB0-BC43-B287-7EE6D75FE27A}">
       <text>
         <r>
           <rPr>
@@ -360,7 +459,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S2" authorId="0" shapeId="0" xr:uid="{518F164D-FDCC-E54D-B2DF-8F453ECB1431}">
+    <comment ref="U2" authorId="0" shapeId="0" xr:uid="{518F164D-FDCC-E54D-B2DF-8F453ECB1431}">
       <text>
         <r>
           <rPr>
@@ -393,7 +492,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T2" authorId="0" shapeId="0" xr:uid="{B7D79E05-3555-1641-A199-607AD17F3A98}">
+    <comment ref="V2" authorId="0" shapeId="0" xr:uid="{B7D79E05-3555-1641-A199-607AD17F3A98}">
       <text>
         <r>
           <rPr>
@@ -426,7 +525,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U2" authorId="0" shapeId="0" xr:uid="{EB6F1D42-7F43-8642-AA41-BBF50B143386}">
+    <comment ref="W2" authorId="0" shapeId="0" xr:uid="{EB6F1D42-7F43-8642-AA41-BBF50B143386}">
       <text>
         <r>
           <rPr>
@@ -459,7 +558,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V2" authorId="0" shapeId="0" xr:uid="{AE95BD72-263E-7640-8218-827926A6729F}">
+    <comment ref="X2" authorId="0" shapeId="0" xr:uid="{AE95BD72-263E-7640-8218-827926A6729F}">
       <text>
         <r>
           <rPr>
@@ -492,7 +591,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="W2" authorId="0" shapeId="0" xr:uid="{047D8163-FB8F-4246-99B2-595867513897}">
+    <comment ref="Y2" authorId="0" shapeId="0" xr:uid="{047D8163-FB8F-4246-99B2-595867513897}">
       <text>
         <r>
           <rPr>
@@ -525,7 +624,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="X2" authorId="0" shapeId="0" xr:uid="{7BA8270B-AFA1-CD4D-B70B-0C32B322B130}">
+    <comment ref="Z2" authorId="0" shapeId="0" xr:uid="{7BA8270B-AFA1-CD4D-B70B-0C32B322B130}">
       <text>
         <r>
           <rPr>
@@ -558,7 +657,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Y2" authorId="0" shapeId="0" xr:uid="{726EEEB5-AC80-0243-B610-FEFA2F34A1EB}">
+    <comment ref="AA2" authorId="0" shapeId="0" xr:uid="{726EEEB5-AC80-0243-B610-FEFA2F34A1EB}">
       <text>
         <r>
           <rPr>
@@ -591,7 +690,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E3" authorId="0" shapeId="0" xr:uid="{887A79FC-140D-2443-8496-3599E39BA9B7}">
+    <comment ref="G3" authorId="0" shapeId="0" xr:uid="{887A79FC-140D-2443-8496-3599E39BA9B7}">
       <text>
         <r>
           <rPr>
@@ -624,7 +723,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F3" authorId="0" shapeId="0" xr:uid="{71304EAD-8694-A043-956C-0A2C3D40E024}">
+    <comment ref="H3" authorId="0" shapeId="0" xr:uid="{71304EAD-8694-A043-956C-0A2C3D40E024}">
       <text>
         <r>
           <rPr>
@@ -657,106 +756,107 @@
         </r>
       </text>
     </comment>
-    <comment ref="H3" authorId="0" shapeId="0" xr:uid="{49C83D03-F8EC-0A4D-B9F1-028C82EC8FB7}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Matthew Heun:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>$/MJ</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I3" authorId="0" shapeId="0" xr:uid="{E1AF7B22-FBF5-8F4E-B100-E76FDA62CB3C}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Matthew Heun:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>lumens/kW</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="J3" authorId="0" shapeId="0" xr:uid="{A7BA69FC-7890-0148-8572-5FF6A4FC8660}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Matthew Heun:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>lumens/kW</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="N3" authorId="0" shapeId="0" xr:uid="{2DC2CF3D-CB10-0447-A6BB-E13E504BFF4F}">
+    <comment ref="J3" authorId="0" shapeId="0" xr:uid="{49C83D03-F8EC-0A4D-B9F1-028C82EC8FB7}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>$/kW-hr</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K3" authorId="0" shapeId="0" xr:uid="{3A848E02-53A6-E54E-8E01-9938DB10D028}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>lm-hr/kW-hr</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L3" authorId="0" shapeId="0" xr:uid="{A7BA69FC-7890-0148-8572-5FF6A4FC8660}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>lm-hr/kW-hr</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P3" authorId="0" shapeId="0" xr:uid="{2DC2CF3D-CB10-0447-A6BB-E13E504BFF4F}">
       <text>
         <r>
           <rPr>
@@ -789,7 +889,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O3" authorId="0" shapeId="0" xr:uid="{B210CA66-900D-DB4B-B4C2-AD78BD37EB4D}">
+    <comment ref="Q3" authorId="0" shapeId="0" xr:uid="{B210CA66-900D-DB4B-B4C2-AD78BD37EB4D}">
       <text>
         <r>
           <rPr>
@@ -822,7 +922,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P3" authorId="0" shapeId="0" xr:uid="{ABF2326C-BA2D-BE47-8827-CD63D8839125}">
+    <comment ref="R3" authorId="0" shapeId="0" xr:uid="{ABF2326C-BA2D-BE47-8827-CD63D8839125}">
       <text>
         <r>
           <rPr>
@@ -856,7 +956,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q3" authorId="0" shapeId="0" xr:uid="{38DCB468-6D7F-484A-A8F8-EBEF999C7AED}">
+    <comment ref="S3" authorId="0" shapeId="0" xr:uid="{38DCB468-6D7F-484A-A8F8-EBEF999C7AED}">
       <text>
         <r>
           <rPr>
@@ -889,7 +989,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R3" authorId="0" shapeId="0" xr:uid="{DF64169F-D5C4-EF48-A273-4073182699CB}">
+    <comment ref="T3" authorId="0" shapeId="0" xr:uid="{DF64169F-D5C4-EF48-A273-4073182699CB}">
       <text>
         <r>
           <rPr>
@@ -922,7 +1022,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S3" authorId="0" shapeId="0" xr:uid="{FE70D0C3-F2E6-E243-8896-EB0C92299AD5}">
+    <comment ref="U3" authorId="0" shapeId="0" xr:uid="{FE70D0C3-F2E6-E243-8896-EB0C92299AD5}">
       <text>
         <r>
           <rPr>
@@ -955,7 +1055,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T3" authorId="0" shapeId="0" xr:uid="{FFC2A0D3-7A2D-CE4D-83FD-FDA9B4B45B38}">
+    <comment ref="V3" authorId="0" shapeId="0" xr:uid="{FFC2A0D3-7A2D-CE4D-83FD-FDA9B4B45B38}">
       <text>
         <r>
           <rPr>
@@ -988,7 +1088,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U3" authorId="0" shapeId="0" xr:uid="{28F2D47D-E587-9642-9506-677918A4E61E}">
+    <comment ref="W3" authorId="0" shapeId="0" xr:uid="{28F2D47D-E587-9642-9506-677918A4E61E}">
       <text>
         <r>
           <rPr>
@@ -1021,7 +1121,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V3" authorId="0" shapeId="0" xr:uid="{45DDB177-C1A1-5149-92E1-8111CF45C971}">
+    <comment ref="X3" authorId="0" shapeId="0" xr:uid="{45DDB177-C1A1-5149-92E1-8111CF45C971}">
       <text>
         <r>
           <rPr>
@@ -1054,7 +1154,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="W3" authorId="0" shapeId="0" xr:uid="{29C5D0E3-585B-BC4A-B190-9798E0FAB668}">
+    <comment ref="Y3" authorId="0" shapeId="0" xr:uid="{29C5D0E3-585B-BC4A-B190-9798E0FAB668}">
       <text>
         <r>
           <rPr>
@@ -1087,7 +1187,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="X3" authorId="0" shapeId="0" xr:uid="{17F72B11-97B9-7B48-A64B-18186A392A64}">
+    <comment ref="Z3" authorId="0" shapeId="0" xr:uid="{17F72B11-97B9-7B48-A64B-18186A392A64}">
       <text>
         <r>
           <rPr>
@@ -1120,7 +1220,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Y3" authorId="0" shapeId="0" xr:uid="{5CC62B9E-5447-4747-A121-4B743BE1C195}">
+    <comment ref="AA3" authorId="0" shapeId="0" xr:uid="{5CC62B9E-5447-4747-A121-4B743BE1C195}">
       <text>
         <r>
           <rPr>
@@ -1158,7 +1258,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
   <si>
     <t>Case</t>
   </si>
@@ -1172,9 +1272,6 @@
     <t>k</t>
   </si>
   <si>
-    <t>p_E</t>
-  </si>
-  <si>
     <t>q_dot_s_orig</t>
   </si>
   <si>
@@ -1254,6 +1351,27 @@
   </si>
   <si>
     <t>Lamp</t>
+  </si>
+  <si>
+    <t>energy_engr_unit</t>
+  </si>
+  <si>
+    <t>gal</t>
+  </si>
+  <si>
+    <t>lm-hr</t>
+  </si>
+  <si>
+    <t>service_unit</t>
+  </si>
+  <si>
+    <t>miles</t>
+  </si>
+  <si>
+    <t>kW-hr</t>
+  </si>
+  <si>
+    <t>p_E_engr_units</t>
   </si>
 </sst>
 </file>
@@ -1636,27 +1754,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37C61C24-5EEE-2E43-8BFA-CC2DA9B61850}">
-  <dimension ref="A1:Y3"/>
+  <dimension ref="A1:AA3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="W30" sqref="W30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="4" max="4" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.5" customWidth="1"/>
-    <col min="9" max="9" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="13" customWidth="1"/>
-    <col min="14" max="14" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="16.5" customWidth="1"/>
+    <col min="7" max="7" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="13" customWidth="1"/>
+    <col min="16" max="16" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:27">
       <c r="A1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1668,220 +1788,238 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="F1" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="G1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" t="s">
         <v>3</v>
       </c>
-      <c r="H1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" t="s">
-        <v>16</v>
-      </c>
       <c r="J1" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="K1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" t="s">
         <v>22</v>
-      </c>
-      <c r="L1" t="s">
-        <v>20</v>
       </c>
       <c r="M1" t="s">
         <v>21</v>
       </c>
       <c r="N1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O1" t="s">
+        <v>20</v>
+      </c>
+      <c r="P1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>6</v>
+      </c>
+      <c r="R1" t="s">
+        <v>13</v>
+      </c>
+      <c r="S1" t="s">
+        <v>23</v>
+      </c>
+      <c r="T1" t="s">
+        <v>14</v>
+      </c>
+      <c r="U1" t="s">
+        <v>24</v>
+      </c>
+      <c r="V1" t="s">
         <v>5</v>
       </c>
-      <c r="O1" t="s">
+      <c r="W1" t="s">
+        <v>12</v>
+      </c>
+      <c r="X1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="P1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>24</v>
-      </c>
-      <c r="R1" t="s">
-        <v>15</v>
-      </c>
-      <c r="S1" t="s">
+      <c r="D2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" s="3">
+        <v>126.62163000000001</v>
+      </c>
+      <c r="H2" s="2">
+        <v>3.3893390630606466</v>
+      </c>
+      <c r="I2" s="2">
+        <v>1</v>
+      </c>
+      <c r="J2" s="2">
+        <v>2.21</v>
+      </c>
+      <c r="K2" s="2">
         <v>25</v>
       </c>
-      <c r="T1" t="s">
-        <v>6</v>
-      </c>
-      <c r="U1" t="s">
-        <v>13</v>
-      </c>
-      <c r="V1" t="s">
-        <v>17</v>
-      </c>
-      <c r="W1" t="s">
-        <v>26</v>
-      </c>
-      <c r="X1" t="s">
-        <v>18</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:25">
-      <c r="A2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="3">
-        <v>126.62163000000001</v>
-      </c>
-      <c r="F2" s="2">
-        <v>3.3893390630606466</v>
-      </c>
-      <c r="G2" s="2">
+      <c r="L2" s="2">
+        <v>42</v>
+      </c>
+      <c r="M2" s="2">
+        <v>-0.1</v>
+      </c>
+      <c r="N2" s="2">
         <v>1</v>
       </c>
-      <c r="H2" s="2">
-        <v>1.7453574085249099E-2</v>
-      </c>
-      <c r="I2" s="2">
-        <v>25</v>
-      </c>
-      <c r="J2" s="2">
-        <v>42</v>
-      </c>
-      <c r="K2" s="2">
-        <v>-0.1</v>
-      </c>
-      <c r="L2" s="2">
+      <c r="O2" s="2">
         <v>1</v>
       </c>
-      <c r="M2" s="2">
-        <v>1</v>
-      </c>
-      <c r="N2" s="2">
+      <c r="P2" s="2">
         <v>14425</v>
       </c>
-      <c r="O2" s="2">
+      <c r="Q2" s="2">
         <v>27401.277693029457</v>
       </c>
-      <c r="P2" s="2">
+      <c r="R2" s="2">
         <v>28216.1</v>
-      </c>
-      <c r="Q2" s="2">
-        <v>7</v>
-      </c>
-      <c r="R2" s="1">
-        <v>27523.4</v>
       </c>
       <c r="S2" s="2">
         <v>7</v>
       </c>
-      <c r="T2" s="2">
+      <c r="T2" s="1">
+        <v>27523.4</v>
+      </c>
+      <c r="U2" s="2">
+        <v>7</v>
+      </c>
+      <c r="V2" s="2">
         <v>2861.13425677328</v>
       </c>
-      <c r="U2" s="2">
+      <c r="W2" s="2">
         <v>2774.6681207909455</v>
       </c>
-      <c r="V2">
+      <c r="X2">
         <v>34000</v>
-      </c>
-      <c r="W2">
-        <v>14</v>
-      </c>
-      <c r="X2">
-        <v>40000</v>
       </c>
       <c r="Y2">
         <v>14</v>
       </c>
+      <c r="Z2">
+        <v>40000</v>
+      </c>
+      <c r="AA2">
+        <v>14</v>
+      </c>
     </row>
-    <row r="3" spans="1:25">
+    <row r="3" spans="1:27">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="3">
+      <c r="E3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3" s="3">
         <v>3.6</v>
       </c>
-      <c r="F3" s="2">
+      <c r="H3" s="2">
         <v>3.3893390630606466</v>
       </c>
-      <c r="G3" s="2">
+      <c r="I3" s="2">
         <v>1</v>
       </c>
-      <c r="H3" s="2">
-        <v>3.7638919000000007E-2</v>
-      </c>
-      <c r="I3" s="4">
+      <c r="J3" s="2">
+        <v>0.13550000000000001</v>
+      </c>
+      <c r="K3" s="4">
         <v>8833.3333333333303</v>
       </c>
-      <c r="J3" s="2">
+      <c r="L3" s="2">
         <v>81800</v>
       </c>
-      <c r="K3" s="2">
+      <c r="M3" s="2">
         <v>-0.4</v>
       </c>
-      <c r="L3" s="2">
+      <c r="N3" s="2">
         <v>1</v>
       </c>
-      <c r="M3" s="2">
+      <c r="O3" s="2">
         <v>1</v>
       </c>
-      <c r="N3" s="2">
+      <c r="P3" s="2">
         <v>580350</v>
       </c>
-      <c r="O3" s="2">
+      <c r="Q3" s="2">
         <v>27401.277693029457</v>
       </c>
-      <c r="P3" s="2">
+      <c r="R3" s="2">
         <v>1.88</v>
       </c>
-      <c r="Q3" s="2">
+      <c r="S3" s="2">
         <v>1.8</v>
       </c>
-      <c r="R3" s="2">
+      <c r="T3" s="2">
         <v>1.21</v>
       </c>
-      <c r="S3" s="2">
+      <c r="U3" s="2">
         <v>10</v>
       </c>
-      <c r="T3" s="2">
+      <c r="V3" s="2">
         <v>0</v>
       </c>
-      <c r="U3" s="2">
+      <c r="W3" s="2">
         <v>0</v>
       </c>
-      <c r="V3" s="2">
+      <c r="X3" s="2">
         <v>2.2000000000000002</v>
       </c>
-      <c r="W3" s="2">
+      <c r="Y3" s="2">
         <v>1.8</v>
       </c>
-      <c r="X3" s="2">
+      <c r="Z3" s="2">
         <v>6.5</v>
       </c>
-      <c r="Y3" s="2">
+      <c r="AA3" s="2">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated car uncomp elasticity to -0.2, per PB change.
</commit_message>
<xml_diff>
--- a/data/eeu_data.xlsx
+++ b/data/eeu_data.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/ReboundPaper2019/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FCBB6C5-2C21-CC47-A3CC-6E1244AC14CF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AA671F1-B7F9-6440-BE5C-A6FCBE04755A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="23180" yWindow="460" windowWidth="26260" windowHeight="16940" xr2:uid="{7964B245-1BB5-784B-946F-34F7FEF70238}"/>
   </bookViews>
   <sheets>
     <sheet name="EEU data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1948,7 +1948,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2327,10 +2327,10 @@
   <dimension ref="A1:AA4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="4" max="4" width="16.5" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="16.5" customWidth="1"/>
@@ -2344,7 +2344,7 @@
     <col min="22" max="23" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -2427,7 +2427,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:27">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -2459,7 +2459,7 @@
         <v>2.21</v>
       </c>
       <c r="K2" s="2">
-        <v>-0.1</v>
+        <v>-0.2</v>
       </c>
       <c r="L2" s="2">
         <v>1</v>
@@ -2510,7 +2510,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:27">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -2542,7 +2542,7 @@
         <v>2.21</v>
       </c>
       <c r="K3" s="2">
-        <v>-0.1</v>
+        <v>-0.2</v>
       </c>
       <c r="L3" s="2">
         <v>1</v>
@@ -2593,7 +2593,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:27">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>25</v>
       </c>

</xml_diff>

<commit_message>
Now including an example preferences path graph.
</commit_message>
<xml_diff>
--- a/data/eeu_data.xlsx
+++ b/data/eeu_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/ReboundPaper2019/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AA671F1-B7F9-6440-BE5C-A6FCBE04755A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A50226AC-A1D3-E24F-BD61-ADE6A8A54F4D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23180" yWindow="460" windowWidth="26260" windowHeight="16940" xr2:uid="{7964B245-1BB5-784B-946F-34F7FEF70238}"/>
+    <workbookView xWindow="6940" yWindow="460" windowWidth="26260" windowHeight="16940" xr2:uid="{7964B245-1BB5-784B-946F-34F7FEF70238}"/>
   </bookViews>
   <sheets>
     <sheet name="EEU data" sheetId="1" r:id="rId1"/>
@@ -1948,7 +1948,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2326,11 +2326,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37C61C24-5EEE-2E43-8BFA-CC2DA9B61850}">
   <dimension ref="A1:AA4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="4" max="4" width="16.5" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="16.5" customWidth="1"/>
@@ -2344,7 +2344,7 @@
     <col min="22" max="23" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:27">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -2427,7 +2427,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:27">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -2456,10 +2456,10 @@
         <v>1</v>
       </c>
       <c r="J2" s="2">
-        <v>2.21</v>
+        <v>5</v>
       </c>
       <c r="K2" s="2">
-        <v>-0.2</v>
+        <v>-0.4</v>
       </c>
       <c r="L2" s="2">
         <v>1</v>
@@ -2510,7 +2510,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:27">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -2593,7 +2593,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:27">
       <c r="A4" t="s">
         <v>25</v>
       </c>

</xml_diff>

<commit_message>
Now using lamp as the example.
</commit_message>
<xml_diff>
--- a/data/eeu_data.xlsx
+++ b/data/eeu_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/ReboundPaper2019/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10E9690B-98A1-334C-903D-76171D3E26DF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{787A0BD1-2B79-5141-A249-C98626710882}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2540" yWindow="460" windowWidth="26260" windowHeight="16940" xr2:uid="{7964B245-1BB5-784B-946F-34F7FEF70238}"/>
   </bookViews>
@@ -129,7 +129,569 @@
         </r>
       </text>
     </comment>
-    <comment ref="G2" authorId="0" shapeId="0" xr:uid="{E0C9C690-AFEA-354B-AF29-0C1FEEF99065}">
+    <comment ref="G2" authorId="0" shapeId="0" xr:uid="{249B88D5-8C45-2F49-B897-04C08FC94B9A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>MJ/kW-hr</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H2" authorId="0" shapeId="0" xr:uid="{F21A0D6A-AF4D-A24A-8C3D-124BA23C5EC2}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>MJ/$</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J2" authorId="0" shapeId="0" xr:uid="{C4417519-0893-AD4F-902C-F9E2CE8F9844}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>$/kW-hr</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N2" authorId="0" shapeId="0" xr:uid="{1EE3D0CB-1ACF-AC46-9687-35A69D79DEC3}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>lm-hr/kW-hr</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O2" authorId="0" shapeId="0" xr:uid="{BB58BD49-A718-9D41-AADA-FDA366ECF0AB}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>lm-hr/kW-hr</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P2" authorId="0" shapeId="0" xr:uid="{103026A7-07D0-584E-BD40-A8FD7917079F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Lm-hr/yr</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Q2" authorId="0" shapeId="0" xr:uid="{BA38F982-79E9-1742-A9C0-3CD9F77035BB}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>$/year</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="R2" authorId="0" shapeId="0" xr:uid="{FB0C5E9B-8187-6241-A472-EE92173E41AE}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>$</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="S2" authorId="0" shapeId="0" xr:uid="{0DA7397A-F905-1A43-8CD3-0EC341171AE9}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>year</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="T2" authorId="0" shapeId="0" xr:uid="{267C6984-34ED-C149-AA4B-45EDCF917BC6}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>$</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="U2" authorId="0" shapeId="0" xr:uid="{E4325DB6-2B17-E64E-B67E-4039ECC386FD}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>year</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="V2" authorId="0" shapeId="0" xr:uid="{9B9C601E-788F-B24F-8483-064FAE23D2C7}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>$/year</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="W2" authorId="0" shapeId="0" xr:uid="{0B3A1821-343E-A046-84C1-A43EE53EE234}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>$/year</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="X2" authorId="0" shapeId="0" xr:uid="{BA077B63-1D59-DE46-8B9E-A045A76E395D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>MJ</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Y2" authorId="0" shapeId="0" xr:uid="{C80E81A5-BB38-8344-A6B2-AA6FA5F9F335}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>years</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Z2" authorId="0" shapeId="0" xr:uid="{B1142E16-9D5A-F947-8B83-E5ADE08AC501}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>MJ</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AA2" authorId="0" shapeId="0" xr:uid="{5FC48D65-41E9-E442-8F22-B5DAACE45501}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>years</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G3" authorId="0" shapeId="0" xr:uid="{9482D8EB-43D3-CD42-B9A3-577AD33D043C}">
       <text>
         <r>
           <rPr>
@@ -162,7 +724,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H2" authorId="0" shapeId="0" xr:uid="{92D7A336-F57A-0C48-B18D-1BB6F992C1E6}">
+    <comment ref="H3" authorId="0" shapeId="0" xr:uid="{142CF5A0-F2F7-6049-8D23-3DC70BA56F2B}">
       <text>
         <r>
           <rPr>
@@ -195,7 +757,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J2" authorId="0" shapeId="0" xr:uid="{8B904ACE-93C7-6649-B94C-7C669A03F7FE}">
+    <comment ref="J3" authorId="0" shapeId="0" xr:uid="{212DB243-4B09-8641-8DD9-2C5771F409BE}">
       <text>
         <r>
           <rPr>
@@ -228,7 +790,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N2" authorId="0" shapeId="0" xr:uid="{FDB95C97-F430-E141-8BC3-115D8159112E}">
+    <comment ref="N3" authorId="0" shapeId="0" xr:uid="{BD5F855E-F716-1C40-9BD9-51470AF65E6E}">
       <text>
         <r>
           <rPr>
@@ -261,7 +823,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O2" authorId="0" shapeId="0" xr:uid="{4BDEFC20-0462-5C47-8071-5712690912C0}">
+    <comment ref="O3" authorId="0" shapeId="0" xr:uid="{724ED12C-E3B7-174A-AED0-FF81928555B3}">
       <text>
         <r>
           <rPr>
@@ -294,7 +856,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P2" authorId="0" shapeId="0" xr:uid="{79968522-59FA-3B4E-8377-1E3333D8CD88}">
+    <comment ref="P3" authorId="0" shapeId="0" xr:uid="{2E11DCDD-2255-D142-98F1-B4F74C45A04F}">
       <text>
         <r>
           <rPr>
@@ -327,7 +889,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q2" authorId="0" shapeId="0" xr:uid="{8C71A288-B7D7-D04D-AB23-7D7BB88E01B9}">
+    <comment ref="Q3" authorId="0" shapeId="0" xr:uid="{30C499C2-FCE1-5541-A599-047491F4BB43}">
       <text>
         <r>
           <rPr>
@@ -360,7 +922,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R2" authorId="0" shapeId="0" xr:uid="{27714977-819C-7348-BB24-B0D046F0900B}">
+    <comment ref="R3" authorId="0" shapeId="0" xr:uid="{15643D2B-90F6-2E4E-923B-C7BAE01F5865}">
       <text>
         <r>
           <rPr>
@@ -393,7 +955,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S2" authorId="0" shapeId="0" xr:uid="{4CDF0A56-5408-8149-904E-489355E69BB6}">
+    <comment ref="S3" authorId="0" shapeId="0" xr:uid="{C60C194C-E6D8-714B-8103-E2256CEE5592}">
       <text>
         <r>
           <rPr>
@@ -426,7 +988,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T2" authorId="0" shapeId="0" xr:uid="{E49BD5F6-4916-6440-AF93-05E16628EB71}">
+    <comment ref="T3" authorId="0" shapeId="0" xr:uid="{FF3DF81E-1DB0-BC43-B287-7EE6D75FE27A}">
       <text>
         <r>
           <rPr>
@@ -459,7 +1021,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U2" authorId="0" shapeId="0" xr:uid="{5A5836D5-FADD-CF4F-B207-B642F264C5D0}">
+    <comment ref="U3" authorId="0" shapeId="0" xr:uid="{518F164D-FDCC-E54D-B2DF-8F453ECB1431}">
       <text>
         <r>
           <rPr>
@@ -492,7 +1054,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V2" authorId="0" shapeId="0" xr:uid="{62A4D6E4-A58B-8148-906B-8D4CE70C22C0}">
+    <comment ref="V3" authorId="0" shapeId="0" xr:uid="{B7D79E05-3555-1641-A199-607AD17F3A98}">
       <text>
         <r>
           <rPr>
@@ -525,7 +1087,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="W2" authorId="0" shapeId="0" xr:uid="{682E48FE-638C-3A40-8AAA-6B603730BB3D}">
+    <comment ref="W3" authorId="0" shapeId="0" xr:uid="{EB6F1D42-7F43-8642-AA41-BBF50B143386}">
       <text>
         <r>
           <rPr>
@@ -558,7 +1120,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="X2" authorId="0" shapeId="0" xr:uid="{57AE412C-38EA-8E40-9EE6-585BABC95C8F}">
+    <comment ref="X3" authorId="0" shapeId="0" xr:uid="{AE95BD72-263E-7640-8218-827926A6729F}">
       <text>
         <r>
           <rPr>
@@ -591,7 +1153,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Y2" authorId="0" shapeId="0" xr:uid="{3BAED3FD-15AA-044D-9657-95DD609EEF9F}">
+    <comment ref="Y3" authorId="0" shapeId="0" xr:uid="{047D8163-FB8F-4246-99B2-595867513897}">
       <text>
         <r>
           <rPr>
@@ -624,7 +1186,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Z2" authorId="0" shapeId="0" xr:uid="{28AA827F-1EE4-4E44-9B2A-C863040109FC}">
+    <comment ref="Z3" authorId="0" shapeId="0" xr:uid="{7BA8270B-AFA1-CD4D-B70B-0C32B322B130}">
       <text>
         <r>
           <rPr>
@@ -657,7 +1219,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA2" authorId="0" shapeId="0" xr:uid="{9322C48B-0018-8A47-B404-3045520B86F2}">
+    <comment ref="AA3" authorId="0" shapeId="0" xr:uid="{726EEEB5-AC80-0243-B610-FEFA2F34A1EB}">
       <text>
         <r>
           <rPr>
@@ -690,7 +1252,570 @@
         </r>
       </text>
     </comment>
-    <comment ref="G3" authorId="0" shapeId="0" xr:uid="{9482D8EB-43D3-CD42-B9A3-577AD33D043C}">
+    <comment ref="G4" authorId="0" shapeId="0" xr:uid="{887A79FC-140D-2443-8496-3599E39BA9B7}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>MJ/kW-hr</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H4" authorId="0" shapeId="0" xr:uid="{71304EAD-8694-A043-956C-0A2C3D40E024}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>MJ/$</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J4" authorId="0" shapeId="0" xr:uid="{49C83D03-F8EC-0A4D-B9F1-028C82EC8FB7}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>$/kW-hr</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N4" authorId="0" shapeId="0" xr:uid="{3A848E02-53A6-E54E-8E01-9938DB10D028}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>lm-hr/kW-hr</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O4" authorId="0" shapeId="0" xr:uid="{A7BA69FC-7890-0148-8572-5FF6A4FC8660}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>lm-hr/kW-hr</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P4" authorId="0" shapeId="0" xr:uid="{2DC2CF3D-CB10-0447-A6BB-E13E504BFF4F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Lm-hr/yr</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Q4" authorId="0" shapeId="0" xr:uid="{B210CA66-900D-DB4B-B4C2-AD78BD37EB4D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>$/year</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="R4" authorId="0" shapeId="0" xr:uid="{ABF2326C-BA2D-BE47-8827-CD63D8839125}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>$</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="S4" authorId="0" shapeId="0" xr:uid="{38DCB468-6D7F-484A-A8F8-EBEF999C7AED}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>year</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="T4" authorId="0" shapeId="0" xr:uid="{DF64169F-D5C4-EF48-A273-4073182699CB}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>$</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="U4" authorId="0" shapeId="0" xr:uid="{FE70D0C3-F2E6-E243-8896-EB0C92299AD5}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>year</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="V4" authorId="0" shapeId="0" xr:uid="{FFC2A0D3-7A2D-CE4D-83FD-FDA9B4B45B38}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>$/year</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="W4" authorId="0" shapeId="0" xr:uid="{28F2D47D-E587-9642-9506-677918A4E61E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>$/year</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="X4" authorId="0" shapeId="0" xr:uid="{45DDB177-C1A1-5149-92E1-8111CF45C971}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>MJ</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Y4" authorId="0" shapeId="0" xr:uid="{29C5D0E3-585B-BC4A-B190-9798E0FAB668}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>years</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Z4" authorId="0" shapeId="0" xr:uid="{17F72B11-97B9-7B48-A64B-18186A392A64}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>MJ</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AA4" authorId="0" shapeId="0" xr:uid="{5CC62B9E-5447-4747-A121-4B743BE1C195}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>years</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G5" authorId="0" shapeId="0" xr:uid="{E0C9C690-AFEA-354B-AF29-0C1FEEF99065}">
       <text>
         <r>
           <rPr>
@@ -723,7 +1848,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H3" authorId="0" shapeId="0" xr:uid="{142CF5A0-F2F7-6049-8D23-3DC70BA56F2B}">
+    <comment ref="H5" authorId="0" shapeId="0" xr:uid="{92D7A336-F57A-0C48-B18D-1BB6F992C1E6}">
       <text>
         <r>
           <rPr>
@@ -756,7 +1881,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J3" authorId="0" shapeId="0" xr:uid="{212DB243-4B09-8641-8DD9-2C5771F409BE}">
+    <comment ref="J5" authorId="0" shapeId="0" xr:uid="{8B904ACE-93C7-6649-B94C-7C669A03F7FE}">
       <text>
         <r>
           <rPr>
@@ -789,7 +1914,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N3" authorId="0" shapeId="0" xr:uid="{BD5F855E-F716-1C40-9BD9-51470AF65E6E}">
+    <comment ref="N5" authorId="0" shapeId="0" xr:uid="{FDB95C97-F430-E141-8BC3-115D8159112E}">
       <text>
         <r>
           <rPr>
@@ -822,7 +1947,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O3" authorId="0" shapeId="0" xr:uid="{724ED12C-E3B7-174A-AED0-FF81928555B3}">
+    <comment ref="O5" authorId="0" shapeId="0" xr:uid="{4BDEFC20-0462-5C47-8071-5712690912C0}">
       <text>
         <r>
           <rPr>
@@ -855,7 +1980,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P3" authorId="0" shapeId="0" xr:uid="{2E11DCDD-2255-D142-98F1-B4F74C45A04F}">
+    <comment ref="P5" authorId="0" shapeId="0" xr:uid="{79968522-59FA-3B4E-8377-1E3333D8CD88}">
       <text>
         <r>
           <rPr>
@@ -888,7 +2013,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q3" authorId="0" shapeId="0" xr:uid="{30C499C2-FCE1-5541-A599-047491F4BB43}">
+    <comment ref="Q5" authorId="0" shapeId="0" xr:uid="{8C71A288-B7D7-D04D-AB23-7D7BB88E01B9}">
       <text>
         <r>
           <rPr>
@@ -921,7 +2046,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R3" authorId="0" shapeId="0" xr:uid="{15643D2B-90F6-2E4E-923B-C7BAE01F5865}">
+    <comment ref="R5" authorId="0" shapeId="0" xr:uid="{27714977-819C-7348-BB24-B0D046F0900B}">
       <text>
         <r>
           <rPr>
@@ -954,7 +2079,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S3" authorId="0" shapeId="0" xr:uid="{C60C194C-E6D8-714B-8103-E2256CEE5592}">
+    <comment ref="S5" authorId="0" shapeId="0" xr:uid="{4CDF0A56-5408-8149-904E-489355E69BB6}">
       <text>
         <r>
           <rPr>
@@ -987,7 +2112,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T3" authorId="0" shapeId="0" xr:uid="{FF3DF81E-1DB0-BC43-B287-7EE6D75FE27A}">
+    <comment ref="T5" authorId="0" shapeId="0" xr:uid="{E49BD5F6-4916-6440-AF93-05E16628EB71}">
       <text>
         <r>
           <rPr>
@@ -1020,7 +2145,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U3" authorId="0" shapeId="0" xr:uid="{518F164D-FDCC-E54D-B2DF-8F453ECB1431}">
+    <comment ref="U5" authorId="0" shapeId="0" xr:uid="{5A5836D5-FADD-CF4F-B207-B642F264C5D0}">
       <text>
         <r>
           <rPr>
@@ -1053,7 +2178,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V3" authorId="0" shapeId="0" xr:uid="{B7D79E05-3555-1641-A199-607AD17F3A98}">
+    <comment ref="V5" authorId="0" shapeId="0" xr:uid="{62A4D6E4-A58B-8148-906B-8D4CE70C22C0}">
       <text>
         <r>
           <rPr>
@@ -1086,7 +2211,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="W3" authorId="0" shapeId="0" xr:uid="{EB6F1D42-7F43-8642-AA41-BBF50B143386}">
+    <comment ref="W5" authorId="0" shapeId="0" xr:uid="{682E48FE-638C-3A40-8AAA-6B603730BB3D}">
       <text>
         <r>
           <rPr>
@@ -1119,7 +2244,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="X3" authorId="0" shapeId="0" xr:uid="{AE95BD72-263E-7640-8218-827926A6729F}">
+    <comment ref="X5" authorId="0" shapeId="0" xr:uid="{57AE412C-38EA-8E40-9EE6-585BABC95C8F}">
       <text>
         <r>
           <rPr>
@@ -1152,7 +2277,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Y3" authorId="0" shapeId="0" xr:uid="{047D8163-FB8F-4246-99B2-595867513897}">
+    <comment ref="Y5" authorId="0" shapeId="0" xr:uid="{3BAED3FD-15AA-044D-9657-95DD609EEF9F}">
       <text>
         <r>
           <rPr>
@@ -1185,7 +2310,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Z3" authorId="0" shapeId="0" xr:uid="{7BA8270B-AFA1-CD4D-B70B-0C32B322B130}">
+    <comment ref="Z5" authorId="0" shapeId="0" xr:uid="{28AA827F-1EE4-4E44-9B2A-C863040109FC}">
       <text>
         <r>
           <rPr>
@@ -1218,570 +2343,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA3" authorId="0" shapeId="0" xr:uid="{726EEEB5-AC80-0243-B610-FEFA2F34A1EB}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Matthew Heun:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>years</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G4" authorId="0" shapeId="0" xr:uid="{887A79FC-140D-2443-8496-3599E39BA9B7}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Matthew Heun:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>MJ/kW-hr</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H4" authorId="0" shapeId="0" xr:uid="{71304EAD-8694-A043-956C-0A2C3D40E024}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Matthew Heun:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>MJ/$</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="J4" authorId="0" shapeId="0" xr:uid="{49C83D03-F8EC-0A4D-B9F1-028C82EC8FB7}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Matthew Heun:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>$/kW-hr</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="N4" authorId="0" shapeId="0" xr:uid="{3A848E02-53A6-E54E-8E01-9938DB10D028}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Matthew Heun:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>lm-hr/kW-hr</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="O4" authorId="0" shapeId="0" xr:uid="{A7BA69FC-7890-0148-8572-5FF6A4FC8660}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Matthew Heun:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>lm-hr/kW-hr</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="P4" authorId="0" shapeId="0" xr:uid="{2DC2CF3D-CB10-0447-A6BB-E13E504BFF4F}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Matthew Heun:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Lm-hr/yr</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="Q4" authorId="0" shapeId="0" xr:uid="{B210CA66-900D-DB4B-B4C2-AD78BD37EB4D}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Matthew Heun:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>$/year</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="R4" authorId="0" shapeId="0" xr:uid="{ABF2326C-BA2D-BE47-8827-CD63D8839125}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Matthew Heun:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>$</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="S4" authorId="0" shapeId="0" xr:uid="{38DCB468-6D7F-484A-A8F8-EBEF999C7AED}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Matthew Heun:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>year</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="T4" authorId="0" shapeId="0" xr:uid="{DF64169F-D5C4-EF48-A273-4073182699CB}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Matthew Heun:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>$</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="U4" authorId="0" shapeId="0" xr:uid="{FE70D0C3-F2E6-E243-8896-EB0C92299AD5}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Matthew Heun:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>year</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="V4" authorId="0" shapeId="0" xr:uid="{FFC2A0D3-7A2D-CE4D-83FD-FDA9B4B45B38}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Matthew Heun:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>$/year</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="W4" authorId="0" shapeId="0" xr:uid="{28F2D47D-E587-9642-9506-677918A4E61E}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Matthew Heun:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>$/year</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="X4" authorId="0" shapeId="0" xr:uid="{45DDB177-C1A1-5149-92E1-8111CF45C971}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Matthew Heun:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>MJ</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="Y4" authorId="0" shapeId="0" xr:uid="{29C5D0E3-585B-BC4A-B190-9798E0FAB668}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Matthew Heun:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>years</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="Z4" authorId="0" shapeId="0" xr:uid="{17F72B11-97B9-7B48-A64B-18186A392A64}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Matthew Heun:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>MJ</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AA4" authorId="0" shapeId="0" xr:uid="{5CC62B9E-5447-4747-A121-4B743BE1C195}">
+    <comment ref="AA5" authorId="0" shapeId="0" xr:uid="{9322C48B-0018-8A47-B404-3045520B86F2}">
       <text>
         <r>
           <rPr>
@@ -1819,7 +2381,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="42">
   <si>
     <t>Case</t>
   </si>
@@ -1942,13 +2504,16 @@
   </si>
   <si>
     <t>B</t>
+  </si>
+  <si>
+    <t>Example 2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1982,6 +2547,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -2324,13 +2895,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37C61C24-5EEE-2E43-8BFA-CC2DA9B61850}">
-  <dimension ref="A1:AA4"/>
+  <dimension ref="A1:AA5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="4" max="4" width="16.5" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="16.5" customWidth="1"/>
@@ -2344,7 +2915,7 @@
     <col min="22" max="23" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:27">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -2427,27 +2998,27 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:27">
       <c r="A2" t="s">
         <v>25</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D2" t="s">
-        <v>40</v>
+      <c r="C2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="G2" s="3">
-        <v>126.62163000000001</v>
+        <v>3.6</v>
       </c>
       <c r="H2" s="2">
         <v>3.3893390630606466</v>
@@ -2456,7 +3027,7 @@
         <v>1</v>
       </c>
       <c r="J2" s="2">
-        <v>5</v>
+        <v>0.13550000000000001</v>
       </c>
       <c r="K2" s="2">
         <v>-0.4</v>
@@ -2467,50 +3038,50 @@
       <c r="M2" s="2">
         <v>1</v>
       </c>
-      <c r="N2" s="2">
-        <v>25</v>
+      <c r="N2" s="4">
+        <v>8833.3333333333303</v>
       </c>
       <c r="O2" s="2">
-        <v>28</v>
+        <v>81800</v>
       </c>
       <c r="P2" s="2">
-        <v>14425</v>
+        <v>580350</v>
       </c>
       <c r="Q2" s="2">
-        <v>27401.277693029457</v>
+        <v>200</v>
       </c>
       <c r="R2" s="2">
-        <v>28216.1</v>
+        <v>10</v>
       </c>
       <c r="S2" s="2">
-        <v>7</v>
-      </c>
-      <c r="T2" s="1">
-        <v>27523.4</v>
+        <v>1.8</v>
+      </c>
+      <c r="T2" s="2">
+        <v>1</v>
       </c>
       <c r="U2" s="2">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="V2" s="2">
-        <v>2861.13425677328</v>
+        <v>3</v>
       </c>
       <c r="W2" s="2">
-        <v>2500</v>
-      </c>
-      <c r="X2">
-        <v>34000</v>
-      </c>
-      <c r="Y2">
-        <v>14</v>
-      </c>
-      <c r="Z2">
-        <v>10000</v>
-      </c>
-      <c r="AA2">
-        <v>14</v>
+        <v>0</v>
+      </c>
+      <c r="X2" s="2">
+        <v>20</v>
+      </c>
+      <c r="Y2" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z2" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA2" s="2">
+        <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:27">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -2593,7 +3164,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:27">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -2674,6 +3245,89 @@
       </c>
       <c r="AA4" s="2">
         <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" s="3">
+        <v>126.62163000000001</v>
+      </c>
+      <c r="H5" s="2">
+        <v>3.3893390630606466</v>
+      </c>
+      <c r="I5" s="2">
+        <v>1</v>
+      </c>
+      <c r="J5" s="2">
+        <v>5</v>
+      </c>
+      <c r="K5" s="2">
+        <v>-0.4</v>
+      </c>
+      <c r="L5" s="2">
+        <v>1</v>
+      </c>
+      <c r="M5" s="2">
+        <v>1</v>
+      </c>
+      <c r="N5" s="2">
+        <v>25</v>
+      </c>
+      <c r="O5" s="2">
+        <v>28</v>
+      </c>
+      <c r="P5" s="2">
+        <v>14425</v>
+      </c>
+      <c r="Q5" s="2">
+        <v>27401.277693029457</v>
+      </c>
+      <c r="R5" s="2">
+        <v>28216.1</v>
+      </c>
+      <c r="S5" s="2">
+        <v>7</v>
+      </c>
+      <c r="T5" s="1">
+        <v>27523.4</v>
+      </c>
+      <c r="U5" s="2">
+        <v>7</v>
+      </c>
+      <c r="V5" s="2">
+        <v>2861.13425677328</v>
+      </c>
+      <c r="W5" s="2">
+        <v>2500</v>
+      </c>
+      <c r="X5">
+        <v>34000</v>
+      </c>
+      <c r="Y5">
+        <v>14</v>
+      </c>
+      <c r="Z5">
+        <v>10000</v>
+      </c>
+      <c r="AA5">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working on W-hr and graphs.
</commit_message>
<xml_diff>
--- a/data/eeu_data.xlsx
+++ b/data/eeu_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/ReboundPaper2019/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5B7ADE5-A912-A24D-A9FA-7A22446F3B20}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4106F989-F1F6-EB4F-AC1D-11E730DEDE3D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2540" yWindow="460" windowWidth="26260" windowHeight="16940" xr2:uid="{7964B245-1BB5-784B-946F-34F7FEF70238}"/>
   </bookViews>
@@ -1252,7 +1252,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G4" authorId="0" shapeId="0" xr:uid="{887A79FC-140D-2443-8496-3599E39BA9B7}">
+    <comment ref="G4" authorId="0" shapeId="0" xr:uid="{2932DBC1-621B-534D-B4EE-900AE23244E6}">
       <text>
         <r>
           <rPr>
@@ -1285,7 +1285,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H4" authorId="0" shapeId="0" xr:uid="{71304EAD-8694-A043-956C-0A2C3D40E024}">
+    <comment ref="H4" authorId="0" shapeId="0" xr:uid="{1BCAA372-BE95-DB4E-905F-73371CC94C60}">
       <text>
         <r>
           <rPr>
@@ -1318,7 +1318,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J4" authorId="0" shapeId="0" xr:uid="{49C83D03-F8EC-0A4D-B9F1-028C82EC8FB7}">
+    <comment ref="J4" authorId="0" shapeId="0" xr:uid="{7907893A-A506-0941-8E74-003BDF954802}">
       <text>
         <r>
           <rPr>
@@ -1351,7 +1351,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N4" authorId="0" shapeId="0" xr:uid="{3A848E02-53A6-E54E-8E01-9938DB10D028}">
+    <comment ref="N4" authorId="0" shapeId="0" xr:uid="{5576D8D6-FB4A-CE4F-8C27-8B2CE32F4D56}">
       <text>
         <r>
           <rPr>
@@ -1384,7 +1384,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O4" authorId="0" shapeId="0" xr:uid="{A7BA69FC-7890-0148-8572-5FF6A4FC8660}">
+    <comment ref="O4" authorId="0" shapeId="0" xr:uid="{FADEFDFC-C653-524A-B4E1-DB81FCDB056B}">
       <text>
         <r>
           <rPr>
@@ -1418,7 +1418,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P4" authorId="0" shapeId="0" xr:uid="{2DC2CF3D-CB10-0447-A6BB-E13E504BFF4F}">
+    <comment ref="P4" authorId="0" shapeId="0" xr:uid="{030802E3-3B22-2247-921D-39E93C1EDD63}">
       <text>
         <r>
           <rPr>
@@ -1451,7 +1451,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q4" authorId="0" shapeId="0" xr:uid="{B210CA66-900D-DB4B-B4C2-AD78BD37EB4D}">
+    <comment ref="Q4" authorId="0" shapeId="0" xr:uid="{E42F95D1-5A15-A44D-8B6C-EFCBF705726A}">
       <text>
         <r>
           <rPr>
@@ -1484,7 +1484,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R4" authorId="0" shapeId="0" xr:uid="{ABF2326C-BA2D-BE47-8827-CD63D8839125}">
+    <comment ref="R4" authorId="0" shapeId="0" xr:uid="{85A6A5F6-A2BE-CA4B-9A5D-5C2B643D5188}">
       <text>
         <r>
           <rPr>
@@ -1518,7 +1518,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S4" authorId="0" shapeId="0" xr:uid="{38DCB468-6D7F-484A-A8F8-EBEF999C7AED}">
+    <comment ref="S4" authorId="0" shapeId="0" xr:uid="{DDB014C5-A2CC-FC47-AB30-9F51ABE81900}">
       <text>
         <r>
           <rPr>
@@ -1551,7 +1551,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T4" authorId="0" shapeId="0" xr:uid="{DF64169F-D5C4-EF48-A273-4073182699CB}">
+    <comment ref="T4" authorId="0" shapeId="0" xr:uid="{F75309F3-B254-6B42-ACF3-EB7B62070C9A}">
       <text>
         <r>
           <rPr>
@@ -1584,7 +1584,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U4" authorId="0" shapeId="0" xr:uid="{FE70D0C3-F2E6-E243-8896-EB0C92299AD5}">
+    <comment ref="U4" authorId="0" shapeId="0" xr:uid="{FCC815E5-11DC-7845-9B83-107B9BB0833E}">
       <text>
         <r>
           <rPr>
@@ -1617,7 +1617,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V4" authorId="0" shapeId="0" xr:uid="{FFC2A0D3-7A2D-CE4D-83FD-FDA9B4B45B38}">
+    <comment ref="V4" authorId="0" shapeId="0" xr:uid="{8841F362-90D3-8C4C-AC8E-5C78D027A50A}">
       <text>
         <r>
           <rPr>
@@ -1650,7 +1650,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="W4" authorId="0" shapeId="0" xr:uid="{28F2D47D-E587-9642-9506-677918A4E61E}">
+    <comment ref="W4" authorId="0" shapeId="0" xr:uid="{99786566-807D-2141-B3D8-EC9C23CFBD56}">
       <text>
         <r>
           <rPr>
@@ -1683,7 +1683,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="X4" authorId="0" shapeId="0" xr:uid="{45DDB177-C1A1-5149-92E1-8111CF45C971}">
+    <comment ref="X4" authorId="0" shapeId="0" xr:uid="{4DF8FA29-C568-E543-91D3-01421B5896B3}">
       <text>
         <r>
           <rPr>
@@ -1716,7 +1716,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Y4" authorId="0" shapeId="0" xr:uid="{29C5D0E3-585B-BC4A-B190-9798E0FAB668}">
+    <comment ref="Y4" authorId="0" shapeId="0" xr:uid="{2881D54C-6A08-2541-9F80-637268D2285C}">
       <text>
         <r>
           <rPr>
@@ -1749,7 +1749,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Z4" authorId="0" shapeId="0" xr:uid="{17F72B11-97B9-7B48-A64B-18186A392A64}">
+    <comment ref="Z4" authorId="0" shapeId="0" xr:uid="{35E3A805-B627-0643-B8CC-944CC619506C}">
       <text>
         <r>
           <rPr>
@@ -1782,7 +1782,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA4" authorId="0" shapeId="0" xr:uid="{5CC62B9E-5447-4747-A121-4B743BE1C195}">
+    <comment ref="AA4" authorId="0" shapeId="0" xr:uid="{8C08D8AD-E643-AD46-9778-37D19F8C80AE}">
       <text>
         <r>
           <rPr>
@@ -1820,7 +1820,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="40">
   <si>
     <t>Case</t>
   </si>
@@ -1937,6 +1937,9 @@
   </si>
   <si>
     <t>Example</t>
+  </si>
+  <si>
+    <t>W-hr</t>
   </si>
 </sst>
 </file>
@@ -2328,7 +2331,7 @@
   <dimension ref="A1:AA4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L5" sqref="A5:XFD5"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2611,10 +2614,10 @@
         <v>30</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="G4" s="3">
-        <v>3.6</v>
+        <v>3.5999999999999999E-3</v>
       </c>
       <c r="H4" s="2">
         <v>3.3893390630606466</v>
@@ -2623,7 +2626,7 @@
         <v>1</v>
       </c>
       <c r="J4" s="2">
-        <v>0.13550000000000001</v>
+        <v>1.3549999999999999E-4</v>
       </c>
       <c r="K4" s="2">
         <v>-0.4</v>
@@ -2635,10 +2638,10 @@
         <v>1</v>
       </c>
       <c r="N4" s="4">
-        <v>8833.3333333333303</v>
+        <v>8.8333333333333304</v>
       </c>
       <c r="O4" s="2">
-        <v>81800</v>
+        <v>81.8</v>
       </c>
       <c r="P4" s="2">
         <v>580350</v>

</xml_diff>

<commit_message>
Back to kW-hr for electricity units.
</commit_message>
<xml_diff>
--- a/data/eeu_data.xlsx
+++ b/data/eeu_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/ReboundPaper2019/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matt/github/ReboundPaper2019/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4106F989-F1F6-EB4F-AC1D-11E730DEDE3D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAF33FE9-7D79-DE44-92CA-A192F4FD99D6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2540" yWindow="460" windowWidth="26260" windowHeight="16940" xr2:uid="{7964B245-1BB5-784B-946F-34F7FEF70238}"/>
   </bookViews>
@@ -1351,7 +1351,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N4" authorId="0" shapeId="0" xr:uid="{5576D8D6-FB4A-CE4F-8C27-8B2CE32F4D56}">
+    <comment ref="N4" authorId="0" shapeId="0" xr:uid="{11C1F832-82C4-2E45-81DF-067E46322064}">
       <text>
         <r>
           <rPr>
@@ -1384,7 +1384,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O4" authorId="0" shapeId="0" xr:uid="{FADEFDFC-C653-524A-B4E1-DB81FCDB056B}">
+    <comment ref="O4" authorId="0" shapeId="0" xr:uid="{9C7330C3-CB04-3C48-ACA0-5877345248FF}">
       <text>
         <r>
           <rPr>
@@ -1412,7 +1412,6 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
           <t>lm-hr/kW-hr</t>
         </r>
@@ -1820,7 +1819,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
   <si>
     <t>Case</t>
   </si>
@@ -1937,16 +1936,13 @@
   </si>
   <si>
     <t>Example</t>
-  </si>
-  <si>
-    <t>W-hr</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2328,13 +2324,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37C61C24-5EEE-2E43-8BFA-CC2DA9B61850}">
-  <dimension ref="A1:AA4"/>
+  <dimension ref="A1:AA5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="4" max="4" width="16.5" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="16.5" customWidth="1"/>
@@ -2348,7 +2344,7 @@
     <col min="22" max="23" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -2431,7 +2427,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:27">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -2514,7 +2510,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:27">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -2597,7 +2593,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:27">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -2614,10 +2610,10 @@
         <v>30</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="G4" s="3">
-        <v>3.5999999999999999E-3</v>
+        <v>3.6</v>
       </c>
       <c r="H4" s="2">
         <v>3.3893390630606466</v>
@@ -2626,7 +2622,7 @@
         <v>1</v>
       </c>
       <c r="J4" s="2">
-        <v>1.3549999999999999E-4</v>
+        <v>0.13550000000000001</v>
       </c>
       <c r="K4" s="2">
         <v>-0.4</v>
@@ -2638,10 +2634,10 @@
         <v>1</v>
       </c>
       <c r="N4" s="4">
-        <v>8.8333333333333304</v>
+        <v>8833.3333333333303</v>
       </c>
       <c r="O4" s="2">
-        <v>81.8</v>
+        <v>81800</v>
       </c>
       <c r="P4" s="2">
         <v>580350</v>
@@ -2679,6 +2675,9 @@
       <c r="AA4" s="2">
         <v>10</v>
       </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="J5" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Edits to prices sensitivity analysis.
</commit_message>
<xml_diff>
--- a/data/eeu_data.xlsx
+++ b/data/eeu_data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matt/github/ReboundPaper2019/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/ReboundPaper2019/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAF33FE9-7D79-DE44-92CA-A192F4FD99D6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE8C55D2-76DF-AD44-B7A8-3DC1806C884F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2540" yWindow="460" windowWidth="26260" windowHeight="16940" xr2:uid="{7964B245-1BB5-784B-946F-34F7FEF70238}"/>
   </bookViews>
@@ -1814,12 +1814,1135 @@
         </r>
       </text>
     </comment>
+    <comment ref="G5" authorId="0" shapeId="0" xr:uid="{4056C48C-C34C-174C-BF77-961BE5037BD3}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>MJ/gallon</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H5" authorId="0" shapeId="0" xr:uid="{A387FE68-8AD7-9F4A-A84F-EA1DBA693073}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>MJ/$</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J5" authorId="0" shapeId="0" xr:uid="{BDA24692-A534-9A48-B3E1-C776B2CA0AF9}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>$/gal</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N5" authorId="0" shapeId="0" xr:uid="{74012865-D5C5-B442-824C-56D91BB5E2E4}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>mi/gallon</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O5" authorId="0" shapeId="0" xr:uid="{E4C9E51F-30E0-9046-9328-B6F7537F8AD2}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>mi/gallon</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P5" authorId="0" shapeId="0" xr:uid="{6F995EC8-6A79-6846-9D97-432E6A087B32}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>mi/yr</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Q5" authorId="0" shapeId="0" xr:uid="{51E45CD5-A395-B248-8E81-BA6B5799ADC8}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>$/year</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="R5" authorId="0" shapeId="0" xr:uid="{577E4404-2864-404B-8CCE-6C644E96580C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>$</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="S5" authorId="0" shapeId="0" xr:uid="{F49AB31C-960A-9547-9947-81A4B07608EE}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>year</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="T5" authorId="0" shapeId="0" xr:uid="{4CBDBD7B-5BF2-E043-AA1C-5E1E1FF54EA9}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>$</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="U5" authorId="0" shapeId="0" xr:uid="{8FF7AA45-0FBB-D64A-905B-F3B136F66C54}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>year</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="V5" authorId="0" shapeId="0" xr:uid="{5E184648-FE58-B641-A34A-0ADD6FDF7F5F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>$/year</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="W5" authorId="0" shapeId="0" xr:uid="{F56383BC-5696-044D-B109-42EC8262A1B4}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>$/year</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="X5" authorId="0" shapeId="0" xr:uid="{19D45708-CD7B-8247-BCE0-4E84383FEA96}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>MJ</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Y5" authorId="0" shapeId="0" xr:uid="{282B7987-5567-E04A-8D32-E930CE7FA9C8}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>years</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Z5" authorId="0" shapeId="0" xr:uid="{E437800C-4DFD-AC41-8098-B5A4689AC3FF}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>MJ</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AA5" authorId="0" shapeId="0" xr:uid="{EDC7D713-6DDC-4A42-9B2D-55BE182647AF}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>years</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G6" authorId="0" shapeId="0" xr:uid="{092F05A1-F2A6-EC43-8F16-C33659FCC227}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>MJ/kW-hr</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H6" authorId="0" shapeId="0" xr:uid="{E5C8D82B-BDB1-DC47-8F7D-41562DAC4A4A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>MJ/$</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J6" authorId="0" shapeId="0" xr:uid="{1F058AB4-123A-C24D-B187-1E385A17C192}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>$/kW-hr</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N6" authorId="0" shapeId="0" xr:uid="{5F7ED516-6A16-8E4A-A748-3A59E4FCCA38}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>lm-hr/kW-hr</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O6" authorId="0" shapeId="0" xr:uid="{8BC783F4-062B-774A-8626-C01D98AA86FB}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>lm-hr/kW-hr</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P6" authorId="0" shapeId="0" xr:uid="{6E45AB07-2780-4343-81A7-5FBBB6A091B1}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Lm-hr/yr</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Q6" authorId="0" shapeId="0" xr:uid="{B4C10F7D-D9F6-9C44-ACEA-AE25D2907BB2}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>$/year</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="R6" authorId="0" shapeId="0" xr:uid="{988D413F-04D0-A448-B93C-0E6C72C4ABE6}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>$</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="S6" authorId="0" shapeId="0" xr:uid="{BAF76ADD-69BA-2848-8289-DB107E768723}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>year</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="T6" authorId="0" shapeId="0" xr:uid="{6557DCD5-3C86-1F41-A9DA-B746D947FAFB}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>$</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="U6" authorId="0" shapeId="0" xr:uid="{0328129B-43CF-8643-8219-AE7727F6A1E9}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>year</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="V6" authorId="0" shapeId="0" xr:uid="{41960BAA-D066-F445-9D8F-B1974FDBE9E9}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>$/year</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="W6" authorId="0" shapeId="0" xr:uid="{60240E64-7507-0743-978C-D1A72091792A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>$/year</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="X6" authorId="0" shapeId="0" xr:uid="{A1F0BA58-1501-8F4C-9FE7-A0A402682788}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>MJ</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Y6" authorId="0" shapeId="0" xr:uid="{0539EDFB-7118-4045-B941-10E5FF9B703A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>years</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Z6" authorId="0" shapeId="0" xr:uid="{9FC449E1-E514-FB42-B0AC-C35D6A7AF47E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>MJ</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AA6" authorId="0" shapeId="0" xr:uid="{8F842682-DEE9-5E41-A460-BED7BB769A84}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>years</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="41">
   <si>
     <t>Case</t>
   </si>
@@ -1936,6 +3059,12 @@
   </si>
   <si>
     <t>Example</t>
+  </si>
+  <si>
+    <t>Car - Germany</t>
+  </si>
+  <si>
+    <t>Lamp - Germany</t>
   </si>
 </sst>
 </file>
@@ -2324,10 +3453,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37C61C24-5EEE-2E43-8BFA-CC2DA9B61850}">
-  <dimension ref="A1:AA5"/>
+  <dimension ref="A1:AA6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2677,7 +3806,170 @@
       </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="J5" s="2"/>
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" s="3">
+        <v>126.62163000000001</v>
+      </c>
+      <c r="H5" s="2">
+        <v>3.3893390630606466</v>
+      </c>
+      <c r="I5" s="2">
+        <v>1</v>
+      </c>
+      <c r="J5" s="2">
+        <v>6.1834509000000004</v>
+      </c>
+      <c r="K5" s="2">
+        <v>-0.2</v>
+      </c>
+      <c r="L5" s="2">
+        <v>1</v>
+      </c>
+      <c r="M5" s="2">
+        <v>1</v>
+      </c>
+      <c r="N5" s="2">
+        <v>25</v>
+      </c>
+      <c r="O5" s="2">
+        <v>42</v>
+      </c>
+      <c r="P5" s="2">
+        <v>14425</v>
+      </c>
+      <c r="Q5" s="2">
+        <v>27401.277693029457</v>
+      </c>
+      <c r="R5" s="2">
+        <v>28216.1</v>
+      </c>
+      <c r="S5" s="2">
+        <v>7</v>
+      </c>
+      <c r="T5" s="1">
+        <v>27523.4</v>
+      </c>
+      <c r="U5" s="2">
+        <v>7</v>
+      </c>
+      <c r="V5" s="2">
+        <v>2861.13425677328</v>
+      </c>
+      <c r="W5" s="2">
+        <v>2774.6681207909455</v>
+      </c>
+      <c r="X5">
+        <v>34000</v>
+      </c>
+      <c r="Y5">
+        <v>14</v>
+      </c>
+      <c r="Z5">
+        <v>40000</v>
+      </c>
+      <c r="AA5">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" s="3">
+        <v>3.6</v>
+      </c>
+      <c r="H6" s="2">
+        <v>3.3893390630606466</v>
+      </c>
+      <c r="I6" s="2">
+        <v>1</v>
+      </c>
+      <c r="J6" s="2">
+        <v>0.36299999999999999</v>
+      </c>
+      <c r="K6" s="2">
+        <v>-0.4</v>
+      </c>
+      <c r="L6" s="2">
+        <v>1</v>
+      </c>
+      <c r="M6" s="2">
+        <v>1</v>
+      </c>
+      <c r="N6" s="4">
+        <v>8833.3333333333303</v>
+      </c>
+      <c r="O6" s="2">
+        <v>81800</v>
+      </c>
+      <c r="P6" s="2">
+        <v>580350</v>
+      </c>
+      <c r="Q6" s="2">
+        <v>27401.277693029457</v>
+      </c>
+      <c r="R6" s="2">
+        <v>1.88</v>
+      </c>
+      <c r="S6" s="2">
+        <v>1.8</v>
+      </c>
+      <c r="T6" s="2">
+        <v>1.21</v>
+      </c>
+      <c r="U6" s="2">
+        <v>10</v>
+      </c>
+      <c r="V6" s="2">
+        <v>0</v>
+      </c>
+      <c r="W6" s="2">
+        <v>0</v>
+      </c>
+      <c r="X6" s="2">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="Y6" s="2">
+        <v>1.8</v>
+      </c>
+      <c r="Z6" s="2">
+        <v>6.5</v>
+      </c>
+      <c r="AA6" s="2">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updating numbers for calcs.
</commit_message>
<xml_diff>
--- a/data/eeu_data.xlsx
+++ b/data/eeu_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/ReboundPaper2019/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE8C55D2-76DF-AD44-B7A8-3DC1806C884F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBE1D8B5-A7BA-0E41-B4C5-35EFA23F1985}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2540" yWindow="460" windowWidth="26260" windowHeight="16940" xr2:uid="{7964B245-1BB5-784B-946F-34F7FEF70238}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="43660" windowHeight="6640" xr2:uid="{7964B245-1BB5-784B-946F-34F7FEF70238}"/>
   </bookViews>
   <sheets>
     <sheet name="EEU data" sheetId="1" r:id="rId1"/>
@@ -1511,7 +1511,6 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
           <t>$</t>
         </r>
@@ -2045,7 +2044,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R5" authorId="0" shapeId="0" xr:uid="{577E4404-2864-404B-8CCE-6C644E96580C}">
+    <comment ref="R5" authorId="0" shapeId="0" xr:uid="{A2765EC5-FFA3-B14B-84FA-BE85A0B46C41}">
       <text>
         <r>
           <rPr>
@@ -3071,6 +3070,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="#,##0.00000"/>
+  </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -3133,12 +3135,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3456,7 +3459,7 @@
   <dimension ref="A1:AA6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="AB3" sqref="AB3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3579,13 +3582,13 @@
         <v>3.6</v>
       </c>
       <c r="H2" s="2">
-        <v>3.3893390630606466</v>
+        <v>3.2380660967337498</v>
       </c>
       <c r="I2" s="2">
         <v>1</v>
       </c>
       <c r="J2" s="2">
-        <v>0.13550000000000001</v>
+        <v>0.12870000000000001</v>
       </c>
       <c r="K2" s="2">
         <v>-0.4</v>
@@ -3662,13 +3665,13 @@
         <v>126.62163000000001</v>
       </c>
       <c r="H3" s="2">
-        <v>3.3893390630606466</v>
+        <v>3.2380660967337498</v>
       </c>
       <c r="I3" s="2">
         <v>1</v>
       </c>
       <c r="J3" s="2">
-        <v>2.21</v>
+        <v>2.63</v>
       </c>
       <c r="K3" s="2">
         <v>-0.2</v>
@@ -3689,25 +3692,25 @@
         <v>14425</v>
       </c>
       <c r="Q3" s="2">
-        <v>27401.277693029457</v>
+        <v>27897.989870000001</v>
       </c>
       <c r="R3" s="2">
-        <v>28216.1</v>
+        <v>33446.43</v>
       </c>
       <c r="S3" s="2">
         <v>7</v>
       </c>
       <c r="T3" s="1">
-        <v>27523.4</v>
+        <v>33037.919999999998</v>
       </c>
       <c r="U3" s="2">
         <v>7</v>
       </c>
-      <c r="V3" s="2">
-        <v>2861.13425677328</v>
-      </c>
-      <c r="W3" s="2">
-        <v>2774.6681207909455</v>
+      <c r="V3" s="5">
+        <v>2730.84854</v>
+      </c>
+      <c r="W3" s="5">
+        <v>2709.6940300000001</v>
       </c>
       <c r="X3">
         <v>34000</v>
@@ -3745,13 +3748,13 @@
         <v>3.6</v>
       </c>
       <c r="H4" s="2">
-        <v>3.3893390630606466</v>
+        <v>3.2380660967337498</v>
       </c>
       <c r="I4" s="2">
         <v>1</v>
       </c>
       <c r="J4" s="2">
-        <v>0.13550000000000001</v>
+        <v>0.12870000000000001</v>
       </c>
       <c r="K4" s="2">
         <v>-0.4</v>
@@ -3772,7 +3775,7 @@
         <v>580350</v>
       </c>
       <c r="Q4" s="2">
-        <v>27401.277693029457</v>
+        <v>27897.989870000001</v>
       </c>
       <c r="R4" s="2">
         <v>1.88</v>
@@ -3828,7 +3831,7 @@
         <v>126.62163000000001</v>
       </c>
       <c r="H5" s="2">
-        <v>3.3893390630606466</v>
+        <v>3.2380660967337498</v>
       </c>
       <c r="I5" s="2">
         <v>1</v>
@@ -3855,25 +3858,25 @@
         <v>14425</v>
       </c>
       <c r="Q5" s="2">
-        <v>27401.277693029457</v>
+        <v>27897.989870000001</v>
       </c>
       <c r="R5" s="2">
-        <v>28216.1</v>
+        <v>33446.43</v>
       </c>
       <c r="S5" s="2">
         <v>7</v>
       </c>
       <c r="T5" s="1">
-        <v>27523.4</v>
+        <v>33037.919999999998</v>
       </c>
       <c r="U5" s="2">
         <v>7</v>
       </c>
-      <c r="V5" s="2">
-        <v>2861.13425677328</v>
-      </c>
-      <c r="W5" s="2">
-        <v>2774.6681207909455</v>
+      <c r="V5" s="5">
+        <v>2730.84854</v>
+      </c>
+      <c r="W5" s="5">
+        <v>2709.6940300000001</v>
       </c>
       <c r="X5">
         <v>34000</v>
@@ -3911,7 +3914,7 @@
         <v>3.6</v>
       </c>
       <c r="H6" s="2">
-        <v>3.3893390630606466</v>
+        <v>3.2380660967337498</v>
       </c>
       <c r="I6" s="2">
         <v>1</v>
@@ -3938,7 +3941,7 @@
         <v>580350</v>
       </c>
       <c r="Q6" s="2">
-        <v>27401.277693029457</v>
+        <v>27897.989870000001</v>
       </c>
       <c r="R6" s="2">
         <v>1.88</v>

</xml_diff>

<commit_message>
Update I_E for example case.
</commit_message>
<xml_diff>
--- a/data/eeu_data.xlsx
+++ b/data/eeu_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/ReboundPaper2019/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{706E96D3-A5E6-F447-B847-4B4A95F4C8EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{927FAE7C-ACA0-8649-B9E0-66000CC25D42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="6380" windowWidth="28800" windowHeight="6640" xr2:uid="{7964B245-1BB5-784B-946F-34F7FEF70238}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="9000" xr2:uid="{7964B245-1BB5-784B-946F-34F7FEF70238}"/>
   </bookViews>
   <sheets>
     <sheet name="EEU data" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,15 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -3458,8 +3467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37C61C24-5EEE-2E43-8BFA-CC2DA9B61850}">
   <dimension ref="A1:AA6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3583,7 +3592,7 @@
         <v>3.6</v>
       </c>
       <c r="H2" s="2">
-        <v>3.2380660967337498</v>
+        <v>3.39</v>
       </c>
       <c r="I2" s="2">
         <v>1</v>

</xml_diff>

<commit_message>
Updated I_E for example.
</commit_message>
<xml_diff>
--- a/data/eeu_data.xlsx
+++ b/data/eeu_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/ReboundPaper2019/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{927FAE7C-ACA0-8649-B9E0-66000CC25D42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97FDD28B-7FEB-BA4A-92BD-68A0B736815F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="9000" xr2:uid="{7964B245-1BB5-784B-946F-34F7FEF70238}"/>
   </bookViews>
@@ -19,15 +19,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -3468,7 +3459,7 @@
   <dimension ref="A1:AA6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3592,7 +3583,7 @@
         <v>3.6</v>
       </c>
       <c r="H2" s="2">
-        <v>3.39</v>
+        <v>3.3893390630606501</v>
       </c>
       <c r="I2" s="2">
         <v>1</v>

</xml_diff>

<commit_message>
Added sssec for CD utility model.
</commit_message>
<xml_diff>
--- a/data/eeu_data.xlsx
+++ b/data/eeu_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/ReboundPaper2019/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97FDD28B-7FEB-BA4A-92BD-68A0B736815F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBBBC733-F717-7049-AAB4-289D02980269}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="9000" xr2:uid="{7964B245-1BB5-784B-946F-34F7FEF70238}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="41540" windowHeight="9080" xr2:uid="{7964B245-1BB5-784B-946F-34F7FEF70238}"/>
   </bookViews>
   <sheets>
     <sheet name="EEU data" sheetId="1" r:id="rId1"/>
@@ -3458,8 +3458,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37C61C24-5EEE-2E43-8BFA-CC2DA9B61850}">
   <dimension ref="A1:AA6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3690,7 +3690,7 @@
         <v>42</v>
       </c>
       <c r="P3" s="2">
-        <v>14425</v>
+        <v>12416</v>
       </c>
       <c r="Q3" s="5">
         <v>27929.825550000001</v>
@@ -3856,7 +3856,7 @@
         <v>42</v>
       </c>
       <c r="P5" s="2">
-        <v>14425</v>
+        <v>12416</v>
       </c>
       <c r="Q5" s="5">
         <v>27929.825550000001</v>

</xml_diff>

<commit_message>
Updated German energy prices.
</commit_message>
<xml_diff>
--- a/data/eeu_data.xlsx
+++ b/data/eeu_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/ReboundPaper2019/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBBBC733-F717-7049-AAB4-289D02980269}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33EE0249-4AB3-3E41-9B26-29A0409EFD3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="41540" windowHeight="9080" xr2:uid="{7964B245-1BB5-784B-946F-34F7FEF70238}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="9080" xr2:uid="{7964B245-1BB5-784B-946F-34F7FEF70238}"/>
   </bookViews>
   <sheets>
     <sheet name="EEU data" sheetId="1" r:id="rId1"/>
@@ -3459,7 +3459,7 @@
   <dimension ref="A1:AA6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="Q5" sqref="Q5"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3838,7 +3838,7 @@
         <v>1</v>
       </c>
       <c r="J5" s="2">
-        <v>6.1834509000000004</v>
+        <v>6.5</v>
       </c>
       <c r="K5" s="2">
         <v>-0.2</v>

</xml_diff>